<commit_message>
fixes typo in attribute description for release
</commit_message>
<xml_diff>
--- a/data-raw/metadata/deer_mill_release_metadata.xlsx
+++ b/data-raw/metadata/deer_mill_release_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-deer-mill-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-deer-mill-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995D67CC-9D5C-6D44-B35D-1549EBE97538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BF49FE-8D55-EE44-87CE-39D7C6807345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="500" windowWidth="25300" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3500" yWindow="760" windowWidth="25300" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>stream</t>
   </si>
   <si>
-    <t>Name of stream where fish releaed</t>
-  </si>
-  <si>
     <t>release_origin</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>Type of mark applied to fish during release trial</t>
+  </si>
+  <si>
+    <t>Name of stream where fish released</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:Z980"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -544,7 +544,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -579,10 +579,10 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>20</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="5" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -709,10 +709,10 @@
     </row>
     <row r="6" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -747,10 +747,10 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>21</v>
@@ -778,10 +778,10 @@
     </row>
     <row r="8" spans="1:26" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>21</v>
@@ -809,10 +809,10 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
@@ -844,10 +844,10 @@
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
@@ -28017,13 +28017,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>